<commit_message>
Tested with new ResidualCapacity calculation
</commit_message>
<xml_diff>
--- a/resources/data/CMO-April-2020-forecasts.xlsx
+++ b/resources/data/CMO-April-2020-forecasts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/feo-esmod-osemosys/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642EBDBF-BDEF-B04B-802D-9CB9E91B52DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6EE9A-5B3F-1D48-965C-3AF9B4F07881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Forecast" sheetId="1" r:id="rId1"/>
@@ -2667,7 +2667,7 @@
   <dimension ref="A1:V326"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6:U8"/>
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3561,11 +3561,13 @@
       <c r="T5" s="78">
         <v>212.3</v>
       </c>
-      <c r="U5" s="17">
-        <v>77.885833333333395</v>
-      </c>
-      <c r="V5" s="17">
-        <v>77.885833333333395</v>
+      <c r="U5" s="77">
+        <f>AVERAGE($P5:$T5)</f>
+        <v>194.24</v>
+      </c>
+      <c r="V5" s="77">
+        <f>AVERAGE($P5:$T5)</f>
+        <v>194.24</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -3617,11 +3619,13 @@
       <c r="T6" s="78">
         <v>80</v>
       </c>
-      <c r="U6" s="20">
-        <v>61.407499999999999</v>
-      </c>
-      <c r="V6" s="20">
-        <v>61.407499999999999</v>
+      <c r="U6" s="77">
+        <f t="shared" ref="U6:V8" si="0">AVERAGE($P6:$T6)</f>
+        <v>76.94</v>
+      </c>
+      <c r="V6" s="77">
+        <f t="shared" si="0"/>
+        <v>76.94</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -3673,11 +3677,13 @@
       <c r="T7" s="78">
         <v>28</v>
       </c>
-      <c r="U7" s="17">
-        <v>4.8023512661927796</v>
-      </c>
-      <c r="V7" s="17">
-        <v>4.8023512661927796</v>
+      <c r="U7" s="77">
+        <f t="shared" si="0"/>
+        <v>23.86</v>
+      </c>
+      <c r="V7" s="77">
+        <f t="shared" si="0"/>
+        <v>23.86</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -3729,11 +3735,13 @@
       <c r="T8" s="78">
         <v>6</v>
       </c>
-      <c r="U8" s="20">
-        <v>2.5658833333333302</v>
-      </c>
-      <c r="V8" s="20">
-        <v>2.5658833333333302</v>
+      <c r="U8" s="77">
+        <f t="shared" si="0"/>
+        <v>4.9399999999999995</v>
+      </c>
+      <c r="V8" s="77">
+        <f t="shared" si="0"/>
+        <v>4.9399999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -7032,10 +7040,12 @@
         <v>212.3</v>
       </c>
       <c r="U87" s="77">
-        <v>212.3</v>
+        <f>AVERAGE($P87:$T87)</f>
+        <v>194.24</v>
       </c>
       <c r="V87" s="77">
-        <v>212.3</v>
+        <f>AVERAGE($P87:$T87)</f>
+        <v>194.24</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -7088,10 +7098,12 @@
         <v>80</v>
       </c>
       <c r="U88" s="77">
-        <v>80</v>
+        <f t="shared" ref="U88:V90" si="1">AVERAGE($P88:$T88)</f>
+        <v>76.94</v>
       </c>
       <c r="V88" s="77">
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>76.94</v>
       </c>
     </row>
     <row r="89" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -7144,10 +7156,12 @@
         <v>28</v>
       </c>
       <c r="U89" s="77">
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>23.86</v>
       </c>
       <c r="V89" s="77">
-        <v>28</v>
+        <f t="shared" si="1"/>
+        <v>23.86</v>
       </c>
     </row>
     <row r="90" spans="1:22" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7200,10 +7214,12 @@
         <v>6</v>
       </c>
       <c r="U90" s="77">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>4.9399999999999995</v>
       </c>
       <c r="V90" s="77">
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>4.9399999999999995</v>
       </c>
     </row>
     <row r="91" spans="1:22" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated docs, data, and config files
</commit_message>
<xml_diff>
--- a/resources/data/CMO-April-2020-forecasts.xlsx
+++ b/resources/data/CMO-April-2020-forecasts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/feo-esmod-osemosys/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A6EE9A-5B3F-1D48-965C-3AF9B4F07881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914E580-0402-1D47-B5C6-FC154EA43D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2666,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V326"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B73" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="P87" sqref="P87:V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="6.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updated data for capacities, costs, and fuel prices
</commit_message>
<xml_diff>
--- a/resources/data/CMO-April-2020-forecasts.xlsx
+++ b/resources/data/CMO-April-2020-forecasts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminuser/Documents/repositories/feo-esmod-osemosys/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F914E580-0402-1D47-B5C6-FC154EA43D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211C42E0-5AB6-324D-95A7-8D3C3EB78D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2666,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V326"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B73" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="P87" sqref="P87:V90"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B79" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="U88" sqref="U88:V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7040,12 +7040,12 @@
         <v>212.3</v>
       </c>
       <c r="U87" s="77">
-        <f>AVERAGE($P87:$T87)</f>
-        <v>194.24</v>
+        <f>AVERAGE($L87:$P87)</f>
+        <v>81.103833324080114</v>
       </c>
       <c r="V87" s="77">
-        <f>AVERAGE($P87:$T87)</f>
-        <v>194.24</v>
+        <f>AVERAGE($L87:$P87)</f>
+        <v>81.103833324080114</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -7098,12 +7098,12 @@
         <v>80</v>
       </c>
       <c r="U88" s="77">
-        <f t="shared" ref="U88:V90" si="1">AVERAGE($P88:$T88)</f>
-        <v>76.94</v>
+        <f>AVERAGE($N88:$R88)</f>
+        <v>68.316421344996257</v>
       </c>
       <c r="V88" s="77">
-        <f t="shared" si="1"/>
-        <v>76.94</v>
+        <f>AVERAGE($N88:$R88)</f>
+        <v>68.316421344996257</v>
       </c>
     </row>
     <row r="89" spans="1:22" ht="18" x14ac:dyDescent="0.2">
@@ -7156,12 +7156,12 @@
         <v>28</v>
       </c>
       <c r="U89" s="77">
-        <f t="shared" si="1"/>
-        <v>23.86</v>
+        <f t="shared" ref="U89:V90" si="1">AVERAGE($N89:$R89)</f>
+        <v>14.334981915140954</v>
       </c>
       <c r="V89" s="77">
         <f t="shared" si="1"/>
-        <v>23.86</v>
+        <v>14.334981915140954</v>
       </c>
     </row>
     <row r="90" spans="1:22" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -7215,11 +7215,11 @@
       </c>
       <c r="U90" s="77">
         <f t="shared" si="1"/>
-        <v>4.9399999999999995</v>
+        <v>3.6358538821219661</v>
       </c>
       <c r="V90" s="77">
         <f t="shared" si="1"/>
-        <v>4.9399999999999995</v>
+        <v>3.6358538821219661</v>
       </c>
     </row>
     <row r="91" spans="1:22" s="36" customFormat="1" ht="18" x14ac:dyDescent="0.2">

</xml_diff>